<commit_message>
se cambia los gráficos
se cambia los gráficos
</commit_message>
<xml_diff>
--- a/Comentartios.xlsx
+++ b/Comentartios.xlsx
@@ -372,42 +372,42 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Nombre</t>
+          <t>Sucursal</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Sucursal</t>
+          <t>CARPETA DE GESTIÓN ELECTRO</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>INFRAESTRUCTURA,  el local se encuentra en condiciones respecto a las luces ,  techos , paredes , pisos , baños, humedad </t>
+          <t>Comentarios Carpeta Electro</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Comentarios Carpeta Electro</t>
+          <t>Comentarios Carpeta Afiliaciones</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Comentarios Carpeta Afiliaciones</t>
+          <t>Comentarios Carpeta Super</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Comentarios Carpeta Super</t>
+          <t>Comentarios Controles de Sucursal</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Comentarios Controles de Sucursal</t>
+          <t>Comentarios Controles de Infraestructura</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Comentarios Controles de Infraestructura</t>
+          <t>Pregunta</t>
         </is>
       </c>
     </row>
@@ -417,35 +417,30 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>sebastian isetta</t>
+          <t>Concordia </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Concordia </t>
+          <t>¿Tiene firmados los objetivos de todos los vendedores?;¿Tiene planificación de trabajo por el desvío de objetivos -mes anterior? (template);¿Tiene cierre y devoluciones realizadas mes anterior?;¿Tiene acta de reuniones de los objetivos BC - BL y GEX?;Comunicación: firma de procesos claves;Tiene el Gerente realizado el check list del día?;</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>si</t>
+          <t>Carpetas ordenadas y firmadas por los colaboradores</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Carpetas ordenadas y firmadas por los colaboradores</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
           <t>Buena semana. Se planifica viaje a Feliciano</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Sin novedades</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Sin novedades</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
         <is>
           <t>Buenas condiciones de la sucursal .</t>
         </is>
@@ -457,40 +452,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>sebastian isetta</t>
+          <t>La paz</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>La paz</t>
+          <t>¿Tiene firmados los objetivos de todos los vendedores?;¿Tiene planificación de trabajo por el desvío de objetivos -mes anterior? (template);¿Tiene acta de reuniones de los objetivos BC - BL y GEX?;¿Tiene cierre y devoluciones realizadas mes anterior?;Comunicación: firma de procesos claves;</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>a medias</t>
+          <t>El chevk list de esta semana falta por encontrarse de vacaciones</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>El chevk list de esta semana falta por encontrarse de vacaciones</t>
+          <t>Se llego al capitándo dela zona</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Se llego al capitándo dela zona</t>
+          <t>Buena cantidad de productos en góndolas</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Buena cantidad de productos en góndolas</t>
+          <t>Se arqueo la caja y no de encontró diferencia fuera de lo estipulado por  procedimiento</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
-        <is>
-          <t>Se arqueo la caja y no de encontró diferencia fuera de lo estipulado por  procedimiento</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
         <is>
           <t>Falta pintar la fachada y ver tema del cartel</t>
         </is>
@@ -502,40 +492,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>sebastian isetta</t>
+          <t>La paz</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>La paz</t>
+          <t>¿Tiene firmados los objetivos de todos los vendedores?;¿Tiene planificación de trabajo por el desvío de objetivos -mes anterior? (template);¿Tiene acta de reuniones de los objetivos BC - BL y GEX?;¿Tiene cierre y devoluciones realizadas mes anterior?;Comunicación: firma de procesos claves;Tiene el Gerente realizado el check list del día?;</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>a medias</t>
+          <t>Se realizó la reunión con los vendedores haciendo hincapié en blister y garantía .</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Se realizó la reunión con los vendedores haciendo hincapié en blister y garantía .</t>
+          <t>Se llego en la zona</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Se llego en la zona</t>
+          <t>Se trabaja firmemente en el colaborador que está en el súper hoy</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Se trabaja firmemente en el colaborador que está en el súper hoy</t>
+          <t>Se trabaja en los procesos y política de crédito</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
-        <is>
-          <t>Se trabaja en los procesos y política de crédito</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
         <is>
           <t>Falta trabajos de pintura</t>
         </is>
@@ -547,20 +532,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Juan Navarro</t>
+          <t>Resistencia </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Resistencia </t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>si</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
+          <t>¿Tiene firmados los objetivos de todos los vendedores?;¿Tiene planificación de trabajo por el desvío de objetivos -mes anterior? (template);¿Tiene acta de reuniones de los objetivos BC - BL y GEX?;¿Tiene cierre y devoluciones realizadas mes anterior?;Comunicación: firma de procesos claves;Tiene el Gerente realizado el check list del día?;</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t xml:space="preserve">Ok en líneas generales_x000D_
 </t>
@@ -573,20 +553,15 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Juan Navarro</t>
+          <t>Saenz peña</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Saenz peña</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>si</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
+          <t>¿Tiene firmados los objetivos de todos los vendedores?;¿Tiene planificación de trabajo por el desvío de objetivos -mes anterior? (template);¿Tiene acta de reuniones de los objetivos BC - BL y GEX?;¿Tiene cierre y devoluciones realizadas mes anterior?;Comunicación: firma de procesos claves;</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Ok</t>
         </is>
@@ -598,20 +573,15 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Juan Navarro</t>
+          <t>Resistencia </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Resistencia </t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>si</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
+          <t>¿Tiene firmados los objetivos de todos los vendedores?;¿Tiene planificación de trabajo por el desvío de objetivos -mes anterior? (template);¿Tiene acta de reuniones de los objetivos BC - BL y GEX?;¿Tiene cierre y devoluciones realizadas mes anterior?;Comunicación: firma de procesos claves;Tiene el Gerente realizado el check list del día?;</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>Ok arqueos y administracion</t>
         </is>
@@ -623,20 +593,15 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Juan Navarro</t>
+          <t>Formosa </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Formosa </t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>a medias</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
+          <t>¿Tiene acta de reuniones de los objetivos BC - BL y GEX?;Comunicación: firma de procesos claves;Tiene el Gerente realizado el check list del día?;</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>Inico de gestion</t>
         </is>

</xml_diff>